<commit_message>
SF: tidied up readme and fixed a simple error
</commit_message>
<xml_diff>
--- a/warhammer_elo_risk_assessment.xlsx
+++ b/warhammer_elo_risk_assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shane\Documents\warhammer_elo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{641F89BF-A37A-4552-9462-9B9A2B7F0A95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3DDFD0-F9DB-4B00-9DB2-2F7E10701CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{2EFD2869-BFFC-4FAF-877A-2E81F4DE0D36}"/>
   </bookViews>
@@ -114,18 +114,6 @@
     <t>Likely</t>
   </si>
   <si>
-    <t>Sitting on chair too long</t>
-  </si>
-  <si>
-    <t>Bad posture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Get up and walk around every 15 mins. </t>
-  </si>
-  <si>
-    <t>Erogonormic equipment, chairs etc</t>
-  </si>
-  <si>
     <t>Possible</t>
   </si>
   <si>
@@ -184,6 +172,18 @@
   </si>
   <si>
     <t>Can be run locally to demonstrate only.</t>
+  </si>
+  <si>
+    <t>Traffic monitored</t>
+  </si>
+  <si>
+    <t>Any input shown in plain text</t>
+  </si>
+  <si>
+    <t>Use HTTPS only, however no sensitve information is being entered at this stage</t>
+  </si>
+  <si>
+    <t>use of secure protocols to avoid data being stolen</t>
   </si>
 </sst>
 </file>
@@ -318,14 +318,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,7 +644,7 @@
   <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -665,13 +665,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
@@ -719,7 +719,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -736,7 +736,7 @@
       <c r="H3" s="10">
         <v>25</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="K3" s="9" t="s">
@@ -783,7 +783,7 @@
       <c r="H4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="13"/>
+      <c r="J4" s="14"/>
       <c r="K4" s="9" t="s">
         <v>24</v>
       </c>
@@ -808,19 +808,19 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>11</v>
@@ -828,7 +828,7 @@
       <c r="H5" s="12">
         <v>4</v>
       </c>
-      <c r="J5" s="13"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="9" t="s">
         <v>25</v>
       </c>
@@ -853,29 +853,29 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H6" s="12">
-        <v>5</v>
-      </c>
-      <c r="J6" s="13"/>
+        <v>3</v>
+      </c>
+      <c r="J6" s="14"/>
       <c r="K6" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="L6" s="8">
         <v>2</v>
@@ -898,19 +898,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>11</v>
@@ -918,9 +918,9 @@
       <c r="H7" s="12">
         <v>4</v>
       </c>
-      <c r="J7" s="13"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="9" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="L7" s="8">
         <v>1</v>
@@ -943,16 +943,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>24</v>
@@ -960,7 +960,7 @@
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="13">
         <v>12</v>
       </c>
     </row>
@@ -969,22 +969,22 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H9" s="11">
         <v>6</v>
@@ -1001,6 +1001,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008536A78E35BDE64A9AD9CCE5DC78DBEC" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="349482cdf5ac31b93258d51842cc578b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3643b69d-905f-4c18-a1fa-f669a1d24531" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1e2a2683aa6b65a5cdcce8bdf2878616" ns2:_="">
     <xsd:import namespace="3643b69d-905f-4c18-a1fa-f669a1d24531"/>
@@ -1170,15 +1179,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1186,6 +1186,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68AF4FA-6C86-4C24-9AB0-65AD4D282361}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEB9C54B-712E-46E5-B739-A9B4D10A0F2E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1203,14 +1211,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A68AF4FA-6C86-4C24-9AB0-65AD4D282361}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{888C558A-737D-4AB2-A5CF-DEA79ED69469}">
   <ds:schemaRefs>

</xml_diff>